<commit_message>
Minor updated at data sheets.
</commit_message>
<xml_diff>
--- a/doc/Experiment results of BLIA.xlsx
+++ b/doc/Experiment results of BLIA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11415" windowHeight="6720" tabRatio="897" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11415" windowHeight="6720" tabRatio="897" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1-Table3" sheetId="1" r:id="rId1"/>
@@ -1356,11 +1356,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="3009088"/>
-        <c:axId val="211487096"/>
+        <c:axId val="127635512"/>
+        <c:axId val="213019992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="3009088"/>
+        <c:axId val="127635512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,7 +1479,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211487096"/>
+        <c:crossAx val="213019992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1487,7 +1487,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="211487096"/>
+        <c:axId val="213019992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1586,7 +1586,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3009088"/>
+        <c:crossAx val="127635512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3009,12 +3009,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="158262312"/>
-        <c:axId val="213421992"/>
-        <c:axId val="213370440"/>
+        <c:axId val="213453720"/>
+        <c:axId val="213453328"/>
+        <c:axId val="214753176"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="158262312"/>
+        <c:axId val="213453720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3099,7 +3099,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213421992"/>
+        <c:crossAx val="213453328"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3107,7 +3107,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213421992"/>
+        <c:axId val="213453328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.25"/>
@@ -3133,12 +3133,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158262312"/>
+        <c:crossAx val="213453720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="213370440"/>
+        <c:axId val="214753176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3222,7 +3222,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213421992"/>
+        <c:crossAx val="213453328"/>
         <c:crosses val="max"/>
       </c:serAx>
       <c:spPr>
@@ -3635,11 +3635,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="213474408"/>
-        <c:axId val="213474800"/>
+        <c:axId val="214399664"/>
+        <c:axId val="214613664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="213474408"/>
+        <c:axId val="214399664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3753,7 +3753,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213474800"/>
+        <c:crossAx val="214613664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3761,7 +3761,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213474800"/>
+        <c:axId val="214613664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.25"/>
@@ -3862,7 +3862,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213474408"/>
+        <c:crossAx val="214399664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4240,11 +4240,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="213475584"/>
-        <c:axId val="213475976"/>
+        <c:axId val="214614448"/>
+        <c:axId val="214614840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="213475584"/>
+        <c:axId val="214614448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4357,7 +4357,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213475976"/>
+        <c:crossAx val="214614840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4365,7 +4365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213475976"/>
+        <c:axId val="214614840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.4"/>
@@ -4466,7 +4466,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213475584"/>
+        <c:crossAx val="214614448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5249,7 +5249,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5473,11 +5472,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="213923960"/>
-        <c:axId val="213924352"/>
+        <c:axId val="214616408"/>
+        <c:axId val="214616800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="213923960"/>
+        <c:axId val="214616408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5524,7 +5523,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5591,7 +5589,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213924352"/>
+        <c:crossAx val="214616800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5599,7 +5597,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213924352"/>
+        <c:axId val="214616800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.30000000000000004"/>
@@ -5633,7 +5631,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5700,7 +5697,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213923960"/>
+        <c:crossAx val="214616408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5714,7 +5711,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5822,7 +5818,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6046,11 +6041,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="213925136"/>
-        <c:axId val="213925528"/>
+        <c:axId val="215353864"/>
+        <c:axId val="215354256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="213925136"/>
+        <c:axId val="215353864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6096,7 +6091,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6163,7 +6157,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213925528"/>
+        <c:crossAx val="215354256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6171,7 +6165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213925528"/>
+        <c:axId val="215354256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.8"/>
@@ -6206,7 +6200,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6273,7 +6266,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213925136"/>
+        <c:crossAx val="215353864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.000000000000001E-2"/>
@@ -6288,7 +6281,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6742,11 +6734,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="211714488"/>
-        <c:axId val="211489552"/>
+        <c:axId val="212685664"/>
+        <c:axId val="212367024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="211714488"/>
+        <c:axId val="212685664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6875,7 +6867,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211489552"/>
+        <c:crossAx val="212367024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6883,7 +6875,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="211489552"/>
+        <c:axId val="212367024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6982,7 +6974,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211714488"/>
+        <c:crossAx val="212685664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7449,11 +7441,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="211776816"/>
-        <c:axId val="211396432"/>
+        <c:axId val="212466520"/>
+        <c:axId val="212466904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="211776816"/>
+        <c:axId val="212466520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7573,7 +7565,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211396432"/>
+        <c:crossAx val="212466904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7581,7 +7573,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="211396432"/>
+        <c:axId val="212466904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7681,7 +7673,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211776816"/>
+        <c:crossAx val="212466520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8149,11 +8141,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="158259568"/>
-        <c:axId val="158260352"/>
+        <c:axId val="213359848"/>
+        <c:axId val="104706664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="158259568"/>
+        <c:axId val="213359848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8283,7 +8275,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158260352"/>
+        <c:crossAx val="104706664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8291,7 +8283,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158260352"/>
+        <c:axId val="104706664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8391,7 +8383,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158259568"/>
+        <c:crossAx val="213359848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9813,12 +9805,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="158261136"/>
-        <c:axId val="158261528"/>
-        <c:axId val="212062856"/>
+        <c:axId val="213455288"/>
+        <c:axId val="213455680"/>
+        <c:axId val="213343000"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="158261136"/>
+        <c:axId val="213455288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9903,7 +9895,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158261528"/>
+        <c:crossAx val="213455680"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9911,7 +9903,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158261528"/>
+        <c:axId val="213455680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.14000000000000001"/>
@@ -9936,12 +9928,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158261136"/>
+        <c:crossAx val="213455288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="212062856"/>
+        <c:axId val="213343000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10025,7 +10017,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158261528"/>
+        <c:crossAx val="213455680"/>
         <c:crosses val="max"/>
       </c:serAx>
       <c:spPr>
@@ -11525,12 +11517,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="212412096"/>
-        <c:axId val="212412488"/>
-        <c:axId val="212455864"/>
+        <c:axId val="213456464"/>
+        <c:axId val="213920808"/>
+        <c:axId val="213924904"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="212412096"/>
+        <c:axId val="213456464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11571,6 +11563,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11615,7 +11608,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212412488"/>
+        <c:crossAx val="213920808"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11623,7 +11616,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="212412488"/>
+        <c:axId val="213920808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.25"/>
@@ -11649,12 +11642,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212412096"/>
+        <c:crossAx val="213456464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="212455864"/>
+        <c:axId val="213924904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11695,6 +11688,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11738,7 +11732,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212412488"/>
+        <c:crossAx val="213920808"/>
         <c:crosses val="max"/>
       </c:serAx>
       <c:spPr>
@@ -11791,6 +11785,27 @@
           </a:p>
         </c:txPr>
       </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13197,12 +13212,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="212413272"/>
-        <c:axId val="212413664"/>
-        <c:axId val="212867728"/>
+        <c:axId val="213921592"/>
+        <c:axId val="213921984"/>
+        <c:axId val="214020040"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="212413272"/>
+        <c:axId val="213921592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13288,7 +13303,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212413664"/>
+        <c:crossAx val="213921984"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13296,7 +13311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="212413664"/>
+        <c:axId val="213921984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.14000000000000001"/>
@@ -13322,12 +13337,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212413272"/>
+        <c:crossAx val="213921592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="212867728"/>
+        <c:axId val="214020040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13412,7 +13427,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212413664"/>
+        <c:crossAx val="213921984"/>
         <c:crosses val="max"/>
       </c:serAx>
       <c:spPr>
@@ -14932,12 +14947,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="212411312"/>
-        <c:axId val="212414448"/>
-        <c:axId val="213122976"/>
+        <c:axId val="213922768"/>
+        <c:axId val="213923160"/>
+        <c:axId val="214455536"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="212411312"/>
+        <c:axId val="213922768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14978,6 +14993,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15022,7 +15038,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212414448"/>
+        <c:crossAx val="213923160"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15030,7 +15046,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="212414448"/>
+        <c:axId val="213923160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.25"/>
@@ -15056,12 +15072,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212411312"/>
+        <c:crossAx val="213922768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="213122976"/>
+        <c:axId val="214455536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15102,6 +15118,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15145,7 +15162,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212414448"/>
+        <c:crossAx val="213923160"/>
         <c:crosses val="max"/>
       </c:serAx>
       <c:spPr>
@@ -15198,6 +15215,67 @@
           </a:p>
         </c:txPr>
       </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16604,12 +16682,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="212411704"/>
-        <c:axId val="158263096"/>
-        <c:axId val="211738744"/>
+        <c:axId val="213454896"/>
+        <c:axId val="213454504"/>
+        <c:axId val="214320856"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="212411704"/>
+        <c:axId val="213454896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16694,7 +16772,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158263096"/>
+        <c:crossAx val="213454504"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16702,7 +16780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158263096"/>
+        <c:axId val="213454504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.14000000000000001"/>
@@ -16728,12 +16806,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212411704"/>
+        <c:crossAx val="213454896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="211738744"/>
+        <c:axId val="214320856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16817,7 +16895,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158263096"/>
+        <c:crossAx val="213454504"/>
         <c:crosses val="max"/>
       </c:serAx>
       <c:spPr>
@@ -24712,8 +24790,8 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -25068,23 +25146,23 @@
         <v>0.1</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:C19" si="10">C10/$C$13</f>
+        <f>C10/$C$13</f>
         <v>9.4736842105263147E-2</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17:D19" si="11">D10/$D$13</f>
+        <f>D10/$D$13</f>
         <v>8.8888888888888906E-2</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17:E19" si="12">E10/$E$13</f>
+        <f>E10/$E$13</f>
         <v>8.2352941176470587E-2</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17:F19" si="13">F10/$F$13</f>
+        <f>F10/$F$13</f>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17:G19" si="14">AVERAGE(B17:F17)</f>
+        <f t="shared" ref="G17:G19" si="10">AVERAGE(B17:F17)</f>
         <v>8.8195734434124526E-2</v>
       </c>
     </row>
@@ -25097,23 +25175,23 @@
         <v>0.5</v>
       </c>
       <c r="C18">
+        <f>C11/$C$13</f>
+        <v>0.47368421052631571</v>
+      </c>
+      <c r="D18">
+        <f>D11/$D$13</f>
+        <v>0.44444444444444448</v>
+      </c>
+      <c r="E18">
+        <f>E11/$E$13</f>
+        <v>0.41176470588235292</v>
+      </c>
+      <c r="F18">
+        <f>F11/$F$13</f>
+        <v>0.37499999999999994</v>
+      </c>
+      <c r="G18">
         <f t="shared" si="10"/>
-        <v>0.47368421052631571</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="11"/>
-        <v>0.44444444444444448</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="12"/>
-        <v>0.41176470588235292</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="13"/>
-        <v>0.37499999999999994</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="14"/>
         <v>0.44097867217062259</v>
       </c>
     </row>
@@ -25126,23 +25204,23 @@
         <v>0</v>
       </c>
       <c r="C19">
+        <f>C12/$C$13</f>
+        <v>5.2631578947368411E-2</v>
+      </c>
+      <c r="D19">
+        <f>D12/$D$13</f>
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="E19">
+        <f>E12/$E$13</f>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="F19">
+        <f>F12/$F$13</f>
+        <v>0.25</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="10"/>
-        <v>5.2631578947368411E-2</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="11"/>
-        <v>0.11111111111111112</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="12"/>
-        <v>0.17647058823529413</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="13"/>
-        <v>0.25</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="14"/>
         <v>0.11804265565875474</v>
       </c>
     </row>
@@ -25152,30 +25230,31 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:G20" si="15">SUM(C16:C19)</f>
+        <f t="shared" ref="C20:G20" si="11">SUM(C16:C19)</f>
         <v>0.99999999999999978</v>
       </c>
       <c r="D20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="E20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="F20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>0.99999999999999989</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -43788,8 +43867,8 @@
   </sheetPr>
   <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>